<commit_message>
chore(runtime): publish files + archive (2025-11-14 15:04:22)
</commit_message>
<xml_diff>
--- a/khl/Form-5_Games_actaul.xlsx
+++ b/khl/Form-5_Games_actaul.xlsx
@@ -614,39 +614,39 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Авангард</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Ак Барс</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>897755</v>
+        <v>897753</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897755.html</t>
+          <t>https://text.khl.ru/text/897753.html</t>
         </is>
       </c>
       <c r="F2" t="n">
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I2" t="n">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="J2" t="n">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="K2" t="n">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -655,57 +655,57 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="O2" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="P2" t="n">
         <v>33</v>
       </c>
       <c r="Q2" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="R2" t="n">
+        <v>17</v>
+      </c>
+      <c r="S2" t="n">
+        <v>6</v>
+      </c>
+      <c r="T2" t="n">
+        <v>41</v>
+      </c>
+      <c r="U2" t="n">
+        <v>30</v>
+      </c>
+      <c r="V2" t="n">
         <v>4</v>
       </c>
-      <c r="S2" t="n">
-        <v>28</v>
-      </c>
-      <c r="T2" t="n">
-        <v>29</v>
-      </c>
-      <c r="U2" t="n">
-        <v>19</v>
-      </c>
-      <c r="V2" t="n">
-        <v>1</v>
-      </c>
       <c r="W2" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="X2" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="Y2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Z2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA2" t="n">
         <v>3</v>
       </c>
-      <c r="AA2" t="n">
-        <v>5</v>
-      </c>
       <c r="AB2" t="inlineStr">
         <is>
           <t>L</t>
         </is>
       </c>
       <c r="AC2" t="n">
-        <v>54.1</v>
+        <v>47.8</v>
       </c>
       <c r="AD2" t="n">
-        <v>60.4</v>
+        <v>57.7</v>
       </c>
       <c r="AE2" t="n">
         <v>0</v>
@@ -717,7 +717,7 @@
         <v>1</v>
       </c>
       <c r="AH2" t="n">
-        <v>0</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="3">
@@ -728,36 +728,36 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Авангард</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>Салават Юлаев</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>897743</v>
+        <v>897741</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897743.html</t>
+          <t>https://text.khl.ru/text/897741.html</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J3" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K3" t="n">
         <v>61</v>
@@ -769,54 +769,54 @@
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P3" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="Q3" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="R3" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="S3" t="n">
         <v>15</v>
       </c>
       <c r="T3" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="U3" t="n">
+        <v>20</v>
+      </c>
+      <c r="V3" t="n">
+        <v>4</v>
+      </c>
+      <c r="W3" t="n">
+        <v>5</v>
+      </c>
+      <c r="X3" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y3" t="n">
         <v>15</v>
       </c>
-      <c r="V3" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" t="n">
+      <c r="Z3" t="n">
         <v>2</v>
       </c>
-      <c r="X3" t="n">
-        <v>15</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>8</v>
-      </c>
-      <c r="Z3" t="n">
+      <c r="AA3" t="n">
         <v>4</v>
       </c>
-      <c r="AA3" t="n">
-        <v>3</v>
-      </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>W</t>
         </is>
       </c>
       <c r="AC3" t="n">
-        <v>63.6</v>
+        <v>47.4</v>
       </c>
       <c r="AD3" t="n">
         <v>58.3</v>
@@ -831,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="AH3" t="n">
-        <v>4.2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -842,338 +842,338 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Авангард</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Трактор</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>897731</v>
+        <v>897734</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897731.html</t>
+          <t>https://text.khl.ru/text/897734.html</t>
         </is>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H4" t="n">
         <v>3</v>
       </c>
       <c r="I4" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="J4" t="n">
         <v>41</v>
       </c>
       <c r="K4" t="n">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="L4" t="n">
         <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
+        <v>4</v>
+      </c>
+      <c r="O4" t="n">
         <v>6</v>
       </c>
-      <c r="O4" t="n">
-        <v>8</v>
-      </c>
       <c r="P4" t="n">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="Q4" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="R4" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="S4" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T4" t="n">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="U4" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="V4" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="W4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="X4" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="Y4" t="n">
         <v>18</v>
       </c>
       <c r="Z4" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="AA4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>W</t>
         </is>
       </c>
       <c r="AC4" t="n">
-        <v>54.4</v>
+        <v>50.9</v>
       </c>
       <c r="AD4" t="n">
-        <v>38.7</v>
+        <v>56.1</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.25</v>
+        <v>0.33</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.25</v>
+        <v>0.33</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AH4" t="n">
-        <v>4.3</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Авангард</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Барыс</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>897718</v>
+        <v>897727</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897718.html</t>
+          <t>https://text.khl.ru/text/897727.html</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
         <v>2</v>
       </c>
-      <c r="H5" t="n">
-        <v>1</v>
-      </c>
       <c r="I5" t="n">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="J5" t="n">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="K5" t="n">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="O5" t="n">
+        <v>8</v>
+      </c>
+      <c r="P5" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>29</v>
+      </c>
+      <c r="R5" t="n">
+        <v>13</v>
+      </c>
+      <c r="S5" t="n">
+        <v>13</v>
+      </c>
+      <c r="T5" t="n">
+        <v>11</v>
+      </c>
+      <c r="U5" t="n">
+        <v>8</v>
+      </c>
+      <c r="V5" t="n">
+        <v>5</v>
+      </c>
+      <c r="W5" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA5" t="n">
         <v>6</v>
       </c>
-      <c r="P5" t="n">
-        <v>30</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>20</v>
-      </c>
-      <c r="R5" t="n">
-        <v>12</v>
-      </c>
-      <c r="S5" t="n">
-        <v>22</v>
-      </c>
-      <c r="T5" t="n">
-        <v>27</v>
-      </c>
-      <c r="U5" t="n">
-        <v>16</v>
-      </c>
-      <c r="V5" t="n">
-        <v>8</v>
-      </c>
-      <c r="W5" t="n">
-        <v>4</v>
-      </c>
-      <c r="X5" t="n">
-        <v>31</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>45</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>6</v>
-      </c>
-      <c r="AA5" t="n">
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="AC5" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>57.9</v>
+      </c>
+      <c r="AE5" t="n">
         <v>3</v>
       </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="AC5" t="n">
-        <v>60</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>62.8</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>1</v>
-      </c>
       <c r="AF5" t="n">
-        <v>0.33</v>
+        <v>0.75</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AH5" t="n">
-        <v>9.5</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Нефтехимик</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>Авангард</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Барыс</t>
-        </is>
-      </c>
       <c r="D6" t="n">
-        <v>897707</v>
+        <v>897718</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897707.html</t>
+          <t>https://text.khl.ru/text/897718.html</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I6" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J6" t="n">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="K6" t="n">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" t="n">
         <v>6</v>
       </c>
       <c r="O6" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="P6" t="n">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q6" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="R6" t="n">
         <v>22</v>
       </c>
       <c r="S6" t="n">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="T6" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="U6" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="V6" t="n">
+        <v>4</v>
+      </c>
+      <c r="W6" t="n">
+        <v>8</v>
+      </c>
+      <c r="X6" t="n">
+        <v>45</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>31</v>
+      </c>
+      <c r="Z6" t="n">
         <v>3</v>
       </c>
-      <c r="W6" t="n">
-        <v>5</v>
-      </c>
-      <c r="X6" t="n">
-        <v>32</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>24</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>2</v>
-      </c>
       <c r="AA6" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC6" t="n">
-        <v>54.4</v>
+        <v>40</v>
       </c>
       <c r="AD6" t="n">
-        <v>58.1</v>
+        <v>37.2</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="AG6" t="n">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="AH6" t="n">
-        <v>13.3</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="7">
@@ -1184,99 +1184,99 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>897753</v>
+        <v>897758</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897753.html</t>
+          <t>https://text.khl.ru/text/897758.html</t>
         </is>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>34</v>
+      </c>
+      <c r="J7" t="n">
+        <v>27</v>
+      </c>
+      <c r="K7" t="n">
+        <v>61</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
         <v>4</v>
       </c>
-      <c r="H7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" t="n">
-        <v>52</v>
-      </c>
-      <c r="J7" t="n">
-        <v>32</v>
-      </c>
-      <c r="K7" t="n">
-        <v>84</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="n">
+      <c r="O7" t="n">
+        <v>4</v>
+      </c>
+      <c r="P7" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>24</v>
+      </c>
+      <c r="R7" t="n">
         <v>9</v>
       </c>
-      <c r="O7" t="n">
-        <v>21</v>
-      </c>
-      <c r="P7" t="n">
-        <v>36</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>33</v>
-      </c>
-      <c r="R7" t="n">
+      <c r="S7" t="n">
+        <v>20</v>
+      </c>
+      <c r="T7" t="n">
         <v>6</v>
       </c>
-      <c r="S7" t="n">
-        <v>17</v>
-      </c>
-      <c r="T7" t="n">
+      <c r="U7" t="n">
+        <v>14</v>
+      </c>
+      <c r="V7" t="n">
+        <v>5</v>
+      </c>
+      <c r="W7" t="n">
+        <v>1</v>
+      </c>
+      <c r="X7" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>28</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="AC7" t="n">
+        <v>53.8</v>
+      </c>
+      <c r="AD7" t="n">
         <v>30</v>
       </c>
-      <c r="U7" t="n">
-        <v>41</v>
-      </c>
-      <c r="V7" t="n">
-        <v>6</v>
-      </c>
-      <c r="W7" t="n">
-        <v>4</v>
-      </c>
-      <c r="X7" t="n">
-        <v>13</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>25</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="AC7" t="n">
-        <v>52.2</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>42.3</v>
-      </c>
       <c r="AE7" t="n">
         <v>0</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="AH7" t="n">
-        <v>7.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1298,110 +1298,107 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Локомотив</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>897745</v>
+        <v>897744</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897745.html</t>
+          <t>https://text.khl.ru/text/897744.html</t>
         </is>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I8" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="J8" t="n">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="K8" t="n">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="L8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
         <v>4</v>
       </c>
       <c r="P8" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>35</v>
+      </c>
+      <c r="R8" t="n">
         <v>19</v>
       </c>
-      <c r="Q8" t="n">
-        <v>26</v>
-      </c>
-      <c r="R8" t="n">
-        <v>20</v>
-      </c>
       <c r="S8" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="T8" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="U8" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="V8" t="n">
         <v>2</v>
       </c>
       <c r="W8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X8" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="Y8" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="Z8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>W</t>
         </is>
       </c>
       <c r="AC8" t="n">
-        <v>42.2</v>
+        <v>39.7</v>
       </c>
       <c r="AD8" t="n">
-        <v>38.6</v>
+        <v>23.7</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AG8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH8" t="n">
-        <v>3.4</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="9">
@@ -1412,110 +1409,110 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Динамо Мн</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>897738</v>
+        <v>897739</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897738.html</t>
+          <t>https://text.khl.ru/text/897739.html</t>
         </is>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H9" t="n">
         <v>4</v>
       </c>
       <c r="I9" t="n">
+        <v>37</v>
+      </c>
+      <c r="J9" t="n">
+        <v>19</v>
+      </c>
+      <c r="K9" t="n">
+        <v>56</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" t="n">
+        <v>2</v>
+      </c>
+      <c r="O9" t="n">
+        <v>8</v>
+      </c>
+      <c r="P9" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q9" t="n">
         <v>26</v>
       </c>
-      <c r="J9" t="n">
-        <v>34</v>
-      </c>
-      <c r="K9" t="n">
-        <v>60</v>
-      </c>
-      <c r="L9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="n">
+      <c r="R9" t="n">
+        <v>9</v>
+      </c>
+      <c r="S9" t="n">
+        <v>14</v>
+      </c>
+      <c r="T9" t="n">
+        <v>10</v>
+      </c>
+      <c r="U9" t="n">
+        <v>33</v>
+      </c>
+      <c r="V9" t="n">
         <v>8</v>
       </c>
-      <c r="O9" t="n">
+      <c r="W9" t="n">
+        <v>10</v>
+      </c>
+      <c r="X9" t="n">
+        <v>26</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>24</v>
+      </c>
+      <c r="Z9" t="n">
         <v>4</v>
       </c>
-      <c r="P9" t="n">
-        <v>43</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>33</v>
-      </c>
-      <c r="R9" t="n">
-        <v>29</v>
-      </c>
-      <c r="S9" t="n">
-        <v>13</v>
-      </c>
-      <c r="T9" t="n">
-        <v>16</v>
-      </c>
-      <c r="U9" t="n">
-        <v>13</v>
-      </c>
-      <c r="V9" t="n">
-        <v>3</v>
-      </c>
-      <c r="W9" t="n">
-        <v>3</v>
-      </c>
-      <c r="X9" t="n">
-        <v>13</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>17</v>
-      </c>
-      <c r="Z9" t="n">
-        <v>8</v>
-      </c>
       <c r="AA9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>W</t>
         </is>
       </c>
       <c r="AC9" t="n">
-        <v>56.6</v>
+        <v>52.7</v>
       </c>
       <c r="AD9" t="n">
-        <v>55.2</v>
+        <v>23.3</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AG9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH9" t="n">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="10">
@@ -1526,20 +1523,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Драконы</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>897716</v>
+        <v>897717</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897716.html</t>
+          <t>https://text.khl.ru/text/897717.html</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -1549,64 +1546,64 @@
         <v>3</v>
       </c>
       <c r="H10" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I10" t="n">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="J10" t="n">
         <v>23</v>
       </c>
       <c r="K10" t="n">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="L10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O10" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P10" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="Q10" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="R10" t="n">
+        <v>16</v>
+      </c>
+      <c r="S10" t="n">
+        <v>18</v>
+      </c>
+      <c r="T10" t="n">
+        <v>14</v>
+      </c>
+      <c r="U10" t="n">
+        <v>28</v>
+      </c>
+      <c r="V10" t="n">
+        <v>2</v>
+      </c>
+      <c r="W10" t="n">
+        <v>1</v>
+      </c>
+      <c r="X10" t="n">
         <v>12</v>
       </c>
-      <c r="S10" t="n">
-        <v>23</v>
-      </c>
-      <c r="T10" t="n">
-        <v>15</v>
-      </c>
-      <c r="U10" t="n">
-        <v>22</v>
-      </c>
-      <c r="V10" t="n">
-        <v>3</v>
-      </c>
-      <c r="W10" t="n">
-        <v>2</v>
-      </c>
-      <c r="X10" t="n">
-        <v>19</v>
-      </c>
       <c r="Y10" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="Z10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AA10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AB10" t="inlineStr">
         <is>
@@ -1614,227 +1611,227 @@
         </is>
       </c>
       <c r="AC10" t="n">
-        <v>65.5</v>
+        <v>53.6</v>
       </c>
       <c r="AD10" t="n">
-        <v>40.5</v>
+        <v>33.3</v>
       </c>
       <c r="AE10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AG10" t="n">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="AH10" t="n">
-        <v>7.3</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Металлург Мг</t>
+          <t>Динамо М</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>897706</v>
+        <v>897708</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897706.html</t>
+          <t>https://text.khl.ru/text/897708.html</t>
         </is>
       </c>
       <c r="F11" t="n">
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I11" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="J11" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="K11" t="n">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="L11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
       </c>
       <c r="N11" t="n">
+        <v>2</v>
+      </c>
+      <c r="O11" t="n">
+        <v>20</v>
+      </c>
+      <c r="P11" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>28</v>
+      </c>
+      <c r="R11" t="n">
         <v>6</v>
       </c>
-      <c r="O11" t="n">
+      <c r="S11" t="n">
+        <v>28</v>
+      </c>
+      <c r="T11" t="n">
+        <v>2</v>
+      </c>
+      <c r="U11" t="n">
+        <v>28</v>
+      </c>
+      <c r="V11" t="n">
+        <v>5</v>
+      </c>
+      <c r="W11" t="n">
+        <v>3</v>
+      </c>
+      <c r="X11" t="n">
+        <v>15</v>
+      </c>
+      <c r="Y11" t="n">
         <v>6</v>
       </c>
-      <c r="P11" t="n">
-        <v>39</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>19</v>
-      </c>
-      <c r="R11" t="n">
-        <v>19</v>
-      </c>
-      <c r="S11" t="n">
+      <c r="Z11" t="n">
         <v>9</v>
       </c>
-      <c r="T11" t="n">
-        <v>18</v>
-      </c>
-      <c r="U11" t="n">
-        <v>11</v>
-      </c>
-      <c r="V11" t="n">
-        <v>4</v>
-      </c>
-      <c r="W11" t="n">
+      <c r="AA11" t="n">
         <v>5</v>
       </c>
-      <c r="X11" t="n">
-        <v>29</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>22</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>7</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>9</v>
-      </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC11" t="n">
-        <v>67.2</v>
+        <v>50</v>
       </c>
       <c r="AD11" t="n">
-        <v>62.1</v>
+        <v>6.7</v>
       </c>
       <c r="AE11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="AG11" t="n">
         <v>1</v>
       </c>
       <c r="AH11" t="n">
-        <v>14.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Динамо М</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Драконы</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>897759</v>
+        <v>897762</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897759.html</t>
+          <t>https://text.khl.ru/text/897762.html</t>
         </is>
       </c>
       <c r="F12" t="n">
         <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H12" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I12" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="J12" t="n">
+        <v>32</v>
+      </c>
+      <c r="K12" t="n">
+        <v>59</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>11</v>
+      </c>
+      <c r="O12" t="n">
         <v>21</v>
       </c>
-      <c r="K12" t="n">
-        <v>56</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>8</v>
-      </c>
       <c r="P12" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="Q12" t="n">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="R12" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="S12" t="n">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="T12" t="n">
+        <v>21</v>
+      </c>
+      <c r="U12" t="n">
         <v>17</v>
-      </c>
-      <c r="U12" t="n">
-        <v>16</v>
       </c>
       <c r="V12" t="n">
         <v>2</v>
       </c>
       <c r="W12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X12" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="Y12" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Z12" t="n">
         <v>4</v>
       </c>
       <c r="AA12" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AB12" t="inlineStr">
         <is>
@@ -1842,133 +1839,136 @@
         </is>
       </c>
       <c r="AC12" t="n">
-        <v>54.7</v>
+        <v>41.9</v>
       </c>
       <c r="AD12" t="n">
-        <v>51.5</v>
+        <v>55.3</v>
       </c>
       <c r="AE12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF12" t="n">
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>1</v>
       </c>
       <c r="AH12" t="n">
-        <v>2.9</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Динамо М</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>897748</v>
+        <v>897752</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897748.html</t>
+          <t>https://text.khl.ru/text/897752.html</t>
         </is>
       </c>
       <c r="F13" t="n">
         <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H13" t="n">
         <v>3</v>
       </c>
       <c r="I13" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="J13" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K13" t="n">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="L13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
         <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O13" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="P13" t="n">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="Q13" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="R13" t="n">
         <v>15</v>
       </c>
       <c r="S13" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="T13" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="U13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W13" t="n">
+        <v>1</v>
+      </c>
+      <c r="X13" t="n">
+        <v>16</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>23</v>
+      </c>
+      <c r="Z13" t="n">
         <v>3</v>
       </c>
-      <c r="X13" t="n">
-        <v>17</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>11</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>2</v>
-      </c>
       <c r="AA13" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>W</t>
         </is>
       </c>
       <c r="AC13" t="n">
-        <v>55.1</v>
+        <v>57.6</v>
       </c>
       <c r="AD13" t="n">
-        <v>57.1</v>
+        <v>55.6</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AG13" t="n">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="AH13" t="n">
-        <v>6.7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -1979,110 +1979,110 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Динамо М</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Лада</t>
+          <t>Локомотив</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>897735</v>
+        <v>897737</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897735.html</t>
+          <t>https://text.khl.ru/text/897737.html</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" t="n">
+        <v>5</v>
+      </c>
+      <c r="I14" t="n">
+        <v>29</v>
+      </c>
+      <c r="J14" t="n">
+        <v>27</v>
+      </c>
+      <c r="K14" t="n">
+        <v>56</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" t="n">
+        <v>6</v>
+      </c>
+      <c r="O14" t="n">
+        <v>8</v>
+      </c>
+      <c r="P14" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>28</v>
+      </c>
+      <c r="R14" t="n">
+        <v>15</v>
+      </c>
+      <c r="S14" t="n">
+        <v>12</v>
+      </c>
+      <c r="T14" t="n">
+        <v>23</v>
+      </c>
+      <c r="U14" t="n">
+        <v>22</v>
+      </c>
+      <c r="V14" t="n">
         <v>3</v>
       </c>
-      <c r="H14" t="n">
+      <c r="W14" t="n">
+        <v>6</v>
+      </c>
+      <c r="X14" t="n">
+        <v>19</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>25</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA14" t="n">
         <v>3</v>
       </c>
-      <c r="I14" t="n">
-        <v>51</v>
-      </c>
-      <c r="J14" t="n">
-        <v>24</v>
-      </c>
-      <c r="K14" t="n">
-        <v>75</v>
-      </c>
-      <c r="L14" t="n">
-        <v>2</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="n">
-        <v>8</v>
-      </c>
-      <c r="O14" t="n">
-        <v>17</v>
-      </c>
-      <c r="P14" t="n">
-        <v>27</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>27</v>
-      </c>
-      <c r="R14" t="n">
-        <v>5</v>
-      </c>
-      <c r="S14" t="n">
-        <v>28</v>
-      </c>
-      <c r="T14" t="n">
-        <v>15</v>
-      </c>
-      <c r="U14" t="n">
-        <v>20</v>
-      </c>
-      <c r="V14" t="n">
-        <v>4</v>
-      </c>
-      <c r="W14" t="n">
-        <v>5</v>
-      </c>
-      <c r="X14" t="n">
-        <v>6</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>8</v>
-      </c>
-      <c r="Z14" t="n">
-        <v>8</v>
-      </c>
-      <c r="AA14" t="n">
-        <v>2</v>
-      </c>
       <c r="AB14" t="inlineStr">
         <is>
           <t>L</t>
         </is>
       </c>
       <c r="AC14" t="n">
-        <v>50</v>
+        <v>46.2</v>
       </c>
       <c r="AD14" t="n">
-        <v>42.9</v>
+        <v>51.1</v>
       </c>
       <c r="AE14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF14" t="n">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="AG14" t="n">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="AH14" t="n">
-        <v>5.9</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="15">
@@ -2093,212 +2093,212 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Динамо М</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>СКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>897726</v>
+        <v>897729</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897726.html</t>
+          <t>https://text.khl.ru/text/897729.html</t>
         </is>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J15" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="K15" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="L15" t="n">
         <v>0</v>
       </c>
       <c r="M15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="O15" t="n">
         <v>8</v>
       </c>
       <c r="P15" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q15" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="R15" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="S15" t="n">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="T15" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="U15" t="n">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="V15" t="n">
+        <v>9</v>
+      </c>
+      <c r="W15" t="n">
+        <v>4</v>
+      </c>
+      <c r="X15" t="n">
+        <v>24</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>32</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA15" t="n">
         <v>3</v>
       </c>
-      <c r="W15" t="n">
-        <v>5</v>
-      </c>
-      <c r="X15" t="n">
-        <v>21</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>30</v>
-      </c>
-      <c r="Z15" t="n">
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="AC15" t="n">
+        <v>52.1</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>44.9</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH15" t="n">
         <v>3</v>
-      </c>
-      <c r="AA15" t="n">
-        <v>4</v>
-      </c>
-      <c r="AB15" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="AC15" t="n">
-        <v>50</v>
-      </c>
-      <c r="AD15" t="n">
-        <v>47.2</v>
-      </c>
-      <c r="AE15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG15" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AH15" t="n">
-        <v>5.6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Динамо М</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ЦСКА</t>
+          <t>ХК Сочи</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>897715</v>
+        <v>897723</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897715.html</t>
+          <t>https://text.khl.ru/text/897723.html</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H16" t="n">
+        <v>5</v>
+      </c>
+      <c r="I16" t="n">
+        <v>50</v>
+      </c>
+      <c r="J16" t="n">
+        <v>30</v>
+      </c>
+      <c r="K16" t="n">
+        <v>80</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
         <v>2</v>
       </c>
-      <c r="I16" t="n">
-        <v>24</v>
-      </c>
-      <c r="J16" t="n">
-        <v>19</v>
-      </c>
-      <c r="K16" t="n">
-        <v>43</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" t="n">
-        <v>1</v>
-      </c>
       <c r="N16" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="O16" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="P16" t="n">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="Q16" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="R16" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="S16" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="T16" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="U16" t="n">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="V16" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W16" t="n">
         <v>4</v>
       </c>
       <c r="X16" t="n">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="Y16" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="Z16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC16" t="n">
-        <v>47.8</v>
+        <v>54.3</v>
       </c>
       <c r="AD16" t="n">
-        <v>59.3</v>
+        <v>43.5</v>
       </c>
       <c r="AE16" t="n">
         <v>0</v>
@@ -2310,50 +2310,50 @@
         <v>0.5</v>
       </c>
       <c r="AH16" t="n">
-        <v>12.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Трактор</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Амур</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>897760</v>
+        <v>897758</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897760.html</t>
+          <t>https://text.khl.ru/text/897758.html</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
         <v>2</v>
       </c>
       <c r="H17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="J17" t="n">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="K17" t="n">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L17" t="n">
         <v>0</v>
@@ -2362,57 +2362,57 @@
         <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O17" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P17" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q17" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R17" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="S17" t="n">
         <v>9</v>
       </c>
       <c r="T17" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="U17" t="n">
         <v>6</v>
       </c>
       <c r="V17" t="n">
+        <v>1</v>
+      </c>
+      <c r="W17" t="n">
+        <v>5</v>
+      </c>
+      <c r="X17" t="n">
+        <v>28</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>31</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA17" t="n">
         <v>2</v>
       </c>
-      <c r="W17" t="n">
-        <v>4</v>
-      </c>
-      <c r="X17" t="n">
-        <v>7</v>
-      </c>
-      <c r="Y17" t="n">
-        <v>16</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>12</v>
-      </c>
-      <c r="AA17" t="n">
-        <v>4</v>
-      </c>
       <c r="AB17" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
       <c r="AC17" t="n">
-        <v>40</v>
+        <v>46.2</v>
       </c>
       <c r="AD17" t="n">
-        <v>53.8</v>
+        <v>70</v>
       </c>
       <c r="AE17" t="n">
         <v>0</v>
@@ -2424,95 +2424,95 @@
         <v>1</v>
       </c>
       <c r="AH17" t="n">
-        <v>5.6</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Трактор</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Адмирал</t>
+          <t>Сибирь</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>897751</v>
+        <v>897746</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897751.html</t>
+          <t>https://text.khl.ru/text/897746.html</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J18" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="K18" t="n">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="L18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M18" t="n">
         <v>0</v>
       </c>
       <c r="N18" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="O18" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P18" t="n">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="Q18" t="n">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="R18" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="S18" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="T18" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U18" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="V18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W18" t="n">
         <v>2</v>
       </c>
       <c r="X18" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="Y18" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA18" t="n">
         <v>1</v>
@@ -2523,71 +2523,68 @@
         </is>
       </c>
       <c r="AC18" t="n">
-        <v>43.3</v>
+        <v>69.8</v>
       </c>
       <c r="AD18" t="n">
-        <v>54.5</v>
+        <v>66.7</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="AF18" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="AG18" t="n">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="AH18" t="n">
-        <v>11.5</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Трактор</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Нефтехимик</t>
+          <t>Торпедо</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>897734</v>
+        <v>897736</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897734.html</t>
+          <t>https://text.khl.ru/text/897736.html</t>
         </is>
       </c>
       <c r="F19" t="n">
         <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I19" t="n">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="J19" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K19" t="n">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="L19" t="n">
         <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19" t="n">
         <v>6</v>
@@ -2596,40 +2593,40 @@
         <v>4</v>
       </c>
       <c r="P19" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="Q19" t="n">
         <v>27</v>
       </c>
       <c r="R19" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S19" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="T19" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="U19" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="V19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W19" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="X19" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="Y19" t="n">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="Z19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB19" t="inlineStr">
         <is>
@@ -2637,10 +2634,10 @@
         </is>
       </c>
       <c r="AC19" t="n">
-        <v>49.1</v>
+        <v>54.2</v>
       </c>
       <c r="AD19" t="n">
-        <v>43.9</v>
+        <v>51.9</v>
       </c>
       <c r="AE19" t="n">
         <v>0</v>
@@ -2649,112 +2646,112 @@
         <v>0</v>
       </c>
       <c r="AG19" t="n">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="AH19" t="n">
-        <v>7.3</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Трактор</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Сибирь</t>
+          <t>Динамо Мн</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>897719</v>
+        <v>897724</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897719.html</t>
+          <t>https://text.khl.ru/text/897724.html</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I20" t="n">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="J20" t="n">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="K20" t="n">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="L20" t="n">
         <v>0</v>
       </c>
       <c r="M20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N20" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O20" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P20" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="Q20" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="R20" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="S20" t="n">
+        <v>21</v>
+      </c>
+      <c r="T20" t="n">
+        <v>12</v>
+      </c>
+      <c r="U20" t="n">
         <v>16</v>
-      </c>
-      <c r="T20" t="n">
-        <v>22</v>
-      </c>
-      <c r="U20" t="n">
-        <v>21</v>
       </c>
       <c r="V20" t="n">
         <v>5</v>
       </c>
       <c r="W20" t="n">
+        <v>1</v>
+      </c>
+      <c r="X20" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>14</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA20" t="n">
         <v>5</v>
       </c>
-      <c r="X20" t="n">
-        <v>18</v>
-      </c>
-      <c r="Y20" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA20" t="n">
-        <v>1</v>
-      </c>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC20" t="n">
-        <v>44.4</v>
+        <v>54.5</v>
       </c>
       <c r="AD20" t="n">
-        <v>51.2</v>
+        <v>42.9</v>
       </c>
       <c r="AE20" t="n">
         <v>0</v>
@@ -2763,124 +2760,124 @@
         <v>0</v>
       </c>
       <c r="AG20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH20" t="n">
-        <v>10.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Трактор</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Барыс</t>
+          <t>Динамо М</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>897712</v>
+        <v>897715</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://text.khl.ru/text/897712.html</t>
+          <t>https://text.khl.ru/text/897715.html</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H21" t="n">
         <v>3</v>
       </c>
       <c r="I21" t="n">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J21" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K21" t="n">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="L21" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
         <v>2</v>
       </c>
-      <c r="M21" t="n">
-        <v>1</v>
-      </c>
-      <c r="N21" t="n">
-        <v>8</v>
-      </c>
       <c r="O21" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="P21" t="n">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="Q21" t="n">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="R21" t="n">
         <v>20</v>
       </c>
       <c r="S21" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="T21" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="U21" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="V21" t="n">
+        <v>4</v>
+      </c>
+      <c r="W21" t="n">
         <v>3</v>
       </c>
-      <c r="W21" t="n">
+      <c r="X21" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>27</v>
+      </c>
+      <c r="Z21" t="n">
         <v>2</v>
       </c>
-      <c r="X21" t="n">
-        <v>29</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>14</v>
-      </c>
-      <c r="Z21" t="n">
-        <v>1</v>
-      </c>
       <c r="AA21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>L</t>
         </is>
       </c>
       <c r="AC21" t="n">
-        <v>56.3</v>
+        <v>52.2</v>
       </c>
       <c r="AD21" t="n">
-        <v>47.8</v>
+        <v>40.7</v>
       </c>
       <c r="AE21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF21" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="AG21" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AH21" t="n">
-        <v>18.2</v>
+        <v>10.5</v>
       </c>
     </row>
   </sheetData>
@@ -3047,353 +3044,353 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Авангард</t>
+          <t>Нефтехимик</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>2.2</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3</v>
+        <v>-0.2</v>
       </c>
       <c r="G2" t="n">
-        <v>32.8</v>
+        <v>28</v>
       </c>
       <c r="H2" t="n">
-        <v>125.7</v>
+        <v>35</v>
       </c>
       <c r="I2" t="n">
-        <v>-2.9</v>
+        <v>0.6</v>
       </c>
       <c r="J2" t="n">
-        <v>34.4</v>
+        <v>37.6</v>
       </c>
       <c r="K2" t="n">
-        <v>34.8</v>
+        <v>124.3</v>
       </c>
       <c r="L2" t="n">
-        <v>1.6</v>
+        <v>-6</v>
       </c>
       <c r="M2" t="n">
-        <v>22.8</v>
+        <v>23.8</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.2</v>
+        <v>-6.7</v>
       </c>
       <c r="O2" t="n">
-        <v>57.3</v>
+        <v>47.72</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.3000000000000007</v>
+        <v>-1.049999999999999</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.166</v>
+        <v>0.236</v>
       </c>
       <c r="R2" t="n">
-        <v>0.083</v>
+        <v>0.09500000000000001</v>
       </c>
       <c r="S2" t="n">
-        <v>0.8460000000000001</v>
+        <v>0.9339999999999999</v>
       </c>
       <c r="T2" t="n">
-        <v>-0.009999999999999998</v>
+        <v>-0.06599999999999999</v>
       </c>
       <c r="U2" t="n">
-        <v>5.4</v>
+        <v>3.4</v>
       </c>
       <c r="V2" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="W2" t="n">
-        <v>9.199999999999999</v>
+        <v>9</v>
       </c>
       <c r="X2" t="n">
-        <v>1.2</v>
+        <v>-3.6</v>
       </c>
       <c r="Y2" t="n">
-        <v>6</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="Z2" t="n">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="AA2" t="n">
-        <v>6.26</v>
+        <v>9.320000000000002</v>
       </c>
       <c r="AB2" t="n">
-        <v>3.19</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ак Барс</t>
+          <t>Северсталь</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>2.4</v>
       </c>
       <c r="D3" t="n">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
       <c r="E3" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.5999999999999999</v>
+      </c>
+      <c r="G3" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="H3" t="n">
+        <v>39.8</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-3.2</v>
+      </c>
+      <c r="J3" t="n">
+        <v>24.4</v>
+      </c>
+      <c r="K3" t="n">
+        <v>89.80000000000001</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-4.2</v>
+      </c>
+      <c r="M3" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-0.3</v>
+      </c>
+      <c r="O3" t="n">
+        <v>49.95999999999999</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.6300000000000004</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.6675</v>
+      </c>
+      <c r="T3" t="n">
+        <v>-0.2209999999999999</v>
+      </c>
+      <c r="U3" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="V3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="W3" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="X3" t="n">
         <v>0.2</v>
       </c>
-      <c r="F3" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>35</v>
-      </c>
-      <c r="H3" t="n">
-        <v>126.5</v>
-      </c>
-      <c r="I3" t="n">
-        <v>-3.8</v>
-      </c>
-      <c r="J3" t="n">
-        <v>29.4</v>
-      </c>
-      <c r="K3" t="n">
-        <v>19.3</v>
-      </c>
-      <c r="L3" t="n">
-        <v>-0.6</v>
-      </c>
-      <c r="M3" t="n">
-        <v>19.2</v>
-      </c>
-      <c r="N3" t="n">
-        <v>-2.6</v>
-      </c>
-      <c r="O3" t="n">
-        <v>56.73999999999999</v>
-      </c>
-      <c r="P3" t="n">
-        <v>5.33</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.316</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.041</v>
-      </c>
-      <c r="S3" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="V3" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="W3" t="n">
-        <v>6.6</v>
-      </c>
-      <c r="X3" t="n">
-        <v>-0.8</v>
-      </c>
       <c r="Y3" t="n">
-        <v>8.6</v>
+        <v>8.4</v>
       </c>
       <c r="Z3" t="n">
-        <v>-2.600000000000001</v>
+        <v>3.4</v>
       </c>
       <c r="AA3" t="n">
-        <v>8.940000000000001</v>
+        <v>7.06</v>
       </c>
       <c r="AB3" t="n">
-        <v>1.81</v>
+        <v>-0.04000000000000004</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Динамо М</t>
+          <t>Спартак</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="D4" t="n">
-        <v>2.6</v>
+        <v>3.8</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4</v>
+        <v>-0.7</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.6</v>
+        <v>-0.5</v>
       </c>
       <c r="G4" t="n">
-        <v>35.2</v>
+        <v>37</v>
       </c>
       <c r="H4" t="n">
-        <v>100.7</v>
+        <v>107.5</v>
       </c>
       <c r="I4" t="n">
-        <v>-1.6</v>
+        <v>3.3</v>
       </c>
       <c r="J4" t="n">
-        <v>23.6</v>
+        <v>28.6</v>
       </c>
       <c r="K4" t="n">
-        <v>20.8</v>
+        <v>7.300000000000001</v>
       </c>
       <c r="L4" t="n">
-        <v>-1.2</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>15.4</v>
+        <v>23</v>
       </c>
       <c r="N4" t="n">
-        <v>0.3</v>
+        <v>3.9</v>
       </c>
       <c r="O4" t="n">
-        <v>51.52</v>
+        <v>50.41999999999999</v>
       </c>
       <c r="P4" t="n">
-        <v>-1.890000000000001</v>
+        <v>1.93</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.08799999999999999</v>
+        <v>0.06999999999999999</v>
       </c>
       <c r="R4" t="n">
         <v>-0.02</v>
       </c>
       <c r="S4" t="n">
-        <v>0.6875</v>
+        <v>0.794</v>
       </c>
       <c r="T4" t="n">
-        <v>-0.04166666666666667</v>
+        <v>-0.08</v>
       </c>
       <c r="U4" t="n">
-        <v>3.8</v>
+        <v>2.6</v>
       </c>
       <c r="V4" t="n">
-        <v>-0.3</v>
+        <v>-0.6</v>
       </c>
       <c r="W4" t="n">
-        <v>4.8</v>
+        <v>8.6</v>
       </c>
       <c r="X4" t="n">
-        <v>0.4</v>
+        <v>-0.8</v>
       </c>
       <c r="Y4" t="n">
-        <v>9</v>
+        <v>10.6</v>
       </c>
       <c r="Z4" t="n">
-        <v>-1.4</v>
+        <v>-2</v>
       </c>
       <c r="AA4" t="n">
-        <v>6.720000000000001</v>
+        <v>7.6</v>
       </c>
       <c r="AB4" t="n">
-        <v>1.81</v>
+        <v>-2.42</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Трактор</t>
+          <t>ЦСКА</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>3.6</v>
+        <v>1.8</v>
       </c>
       <c r="D5" t="n">
-        <v>2.4</v>
+        <v>1.4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9</v>
+        <v>-0.4</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5999999999999999</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="G5" t="n">
-        <v>35</v>
+        <v>26.4</v>
       </c>
       <c r="H5" t="n">
-        <v>34.5</v>
+        <v>20.8</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7</v>
+        <v>-2.1</v>
       </c>
       <c r="J5" t="n">
-        <v>28.6</v>
+        <v>25</v>
       </c>
       <c r="K5" t="n">
-        <v>42.3</v>
+        <v>28</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.1</v>
+        <v>-2.1</v>
       </c>
       <c r="M5" t="n">
-        <v>16.2</v>
+        <v>13</v>
       </c>
       <c r="N5" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="O5" t="n">
+        <v>55.38</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-0.3299999999999997</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.234</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.03299999999999999</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="V5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="W5" t="n">
         <v>4</v>
       </c>
-      <c r="O5" t="n">
-        <v>46.62</v>
-      </c>
-      <c r="P5" t="n">
-        <v>3.37</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.05500000000000001</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.6839999999999999</v>
-      </c>
-      <c r="T5" t="n">
-        <v>-0.15</v>
-      </c>
-      <c r="U5" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="V5" t="n">
-        <v>-2.6</v>
-      </c>
-      <c r="W5" t="n">
-        <v>7.2</v>
-      </c>
       <c r="X5" t="n">
-        <v>-1</v>
+        <v>0.4</v>
       </c>
       <c r="Y5" t="n">
-        <v>6.4</v>
+        <v>4.8</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AA5" t="n">
-        <v>10.58</v>
+        <v>6.840000000000001</v>
       </c>
       <c r="AB5" t="n">
-        <v>2.4</v>
+        <v>-0.6700000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-21 11:04:05)
</commit_message>
<xml_diff>
--- a/khl/Form-5_Games_actaul.xlsx
+++ b/khl/Form-5_Games_actaul.xlsx
@@ -7608,10 +7608,10 @@
         <v>2.8</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.3</v>
+        <v>1.3</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="G2" t="n">
         <v>29.2</v>
@@ -7620,7 +7620,7 @@
         <v>51.2</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.8</v>
+        <v>0.8</v>
       </c>
       <c r="J2" t="n">
         <v>35.8</v>
@@ -7629,55 +7629,55 @@
         <v>14.7</v>
       </c>
       <c r="L2" t="n">
-        <v>0.7</v>
+        <v>-0.7</v>
       </c>
       <c r="M2" t="n">
         <v>11</v>
       </c>
       <c r="N2" t="n">
-        <v>-1.6</v>
+        <v>1.6</v>
       </c>
       <c r="O2" t="n">
         <v>45.26000000000001</v>
       </c>
       <c r="P2" t="n">
-        <v>-2.169999999999999</v>
+        <v>2.169999999999999</v>
       </c>
       <c r="Q2" t="n">
         <v>0.234</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.017</v>
+        <v>0.017</v>
       </c>
       <c r="S2" t="n">
         <v>0.8099999999999999</v>
       </c>
       <c r="T2" t="n">
-        <v>-0.05</v>
+        <v>0.05</v>
       </c>
       <c r="U2" t="n">
         <v>3.6</v>
       </c>
       <c r="V2" t="n">
-        <v>-1.1</v>
+        <v>1.1</v>
       </c>
       <c r="W2" t="n">
         <v>15</v>
       </c>
       <c r="X2" t="n">
-        <v>-0.8</v>
+        <v>0.8</v>
       </c>
       <c r="Y2" t="n">
         <v>5.6</v>
       </c>
       <c r="Z2" t="n">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="AA2" t="n">
         <v>10.64</v>
       </c>
       <c r="AB2" t="n">
-        <v>-3.699999999999999</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="3">
@@ -7696,10 +7696,10 @@
         <v>1.8</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1</v>
+        <v>-0.1</v>
       </c>
       <c r="G3" t="n">
         <v>33.2</v>
@@ -7708,7 +7708,7 @@
         <v>18.7</v>
       </c>
       <c r="I3" t="n">
-        <v>1.6</v>
+        <v>-1.6</v>
       </c>
       <c r="J3" t="n">
         <v>24</v>
@@ -7717,55 +7717,55 @@
         <v>4.5</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="M3" t="n">
         <v>13</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.9</v>
+        <v>0.9</v>
       </c>
       <c r="O3" t="n">
-        <v>52.19999999999999</v>
+        <v>52.2</v>
       </c>
       <c r="P3" t="n">
-        <v>-3.549999999999999</v>
+        <v>3.549999999999999</v>
       </c>
       <c r="Q3" t="n">
         <v>0.05600000000000001</v>
       </c>
       <c r="R3" t="n">
-        <v>-0.017</v>
+        <v>0.017</v>
       </c>
       <c r="S3" t="n">
         <v>0.9</v>
       </c>
       <c r="T3" t="n">
-        <v>0.025</v>
+        <v>-0.025</v>
       </c>
       <c r="U3" t="n">
         <v>7.4</v>
       </c>
       <c r="V3" t="n">
-        <v>-4.4</v>
+        <v>4.4</v>
       </c>
       <c r="W3" t="n">
         <v>6</v>
       </c>
       <c r="X3" t="n">
-        <v>-0.8</v>
+        <v>0.8</v>
       </c>
       <c r="Y3" t="n">
         <v>14.6</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.3999999999999996</v>
+        <v>-0.4</v>
       </c>
       <c r="AA3" t="n">
-        <v>8.479999999999999</v>
+        <v>8.48</v>
       </c>
       <c r="AB3" t="n">
-        <v>-1.14</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="4">
@@ -7784,10 +7784,10 @@
         <v>2.4</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.5000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="G4" t="n">
         <v>30.6</v>
@@ -7796,7 +7796,7 @@
         <v>46.8</v>
       </c>
       <c r="I4" t="n">
-        <v>3.8</v>
+        <v>-3.8</v>
       </c>
       <c r="J4" t="n">
         <v>35.6</v>
@@ -7805,55 +7805,55 @@
         <v>58.3</v>
       </c>
       <c r="L4" t="n">
-        <v>3.5</v>
+        <v>-3.5</v>
       </c>
       <c r="M4" t="n">
         <v>8.4</v>
       </c>
       <c r="N4" t="n">
-        <v>2.5</v>
+        <v>-2.5</v>
       </c>
       <c r="O4" t="n">
         <v>52.06</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.2399999999999999</v>
+        <v>0.2399999999999999</v>
       </c>
       <c r="Q4" t="n">
         <v>0.234</v>
       </c>
       <c r="R4" t="n">
-        <v>0.134</v>
+        <v>-0.134</v>
       </c>
       <c r="S4" t="n">
         <v>0.85</v>
       </c>
       <c r="T4" t="n">
-        <v>-0.04899999999999999</v>
+        <v>0.04899999999999999</v>
       </c>
       <c r="U4" t="n">
         <v>5.6</v>
       </c>
       <c r="V4" t="n">
-        <v>0.8</v>
+        <v>-0.8</v>
       </c>
       <c r="W4" t="n">
         <v>6.8</v>
       </c>
       <c r="X4" t="n">
-        <v>-0.8000000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="Y4" t="n">
         <v>6.4</v>
       </c>
       <c r="Z4" t="n">
-        <v>-0.6</v>
+        <v>0.6</v>
       </c>
       <c r="AA4" t="n">
         <v>6.44</v>
       </c>
       <c r="AB4" t="n">
-        <v>-0.3099999999999999</v>
+        <v>0.3099999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -7872,7 +7872,7 @@
         <v>3.6</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -7884,64 +7884,64 @@
         <v>16.7</v>
       </c>
       <c r="I5" t="n">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
       <c r="J5" t="n">
         <v>29.2</v>
       </c>
       <c r="K5" t="n">
-        <v>22.2</v>
+        <v>22.20000000000001</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.9</v>
+        <v>0.9</v>
       </c>
       <c r="M5" t="n">
         <v>17</v>
       </c>
       <c r="N5" t="n">
-        <v>-1.1</v>
+        <v>1.1</v>
       </c>
       <c r="O5" t="n">
-        <v>48.78</v>
+        <v>48.77999999999999</v>
       </c>
       <c r="P5" t="n">
-        <v>2.73</v>
+        <v>-2.73</v>
       </c>
       <c r="Q5" t="n">
         <v>0.34</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.009999999999999998</v>
+        <v>0.009999999999999998</v>
       </c>
       <c r="S5" t="n">
         <v>0.6875</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.2583333333333334</v>
+        <v>0.008333333333333333</v>
       </c>
       <c r="U5" t="n">
         <v>2.6</v>
       </c>
       <c r="V5" t="n">
-        <v>0.1</v>
+        <v>-0.1</v>
       </c>
       <c r="W5" t="n">
         <v>4.4</v>
       </c>
       <c r="X5" t="n">
-        <v>-0.4</v>
+        <v>0.4</v>
       </c>
       <c r="Y5" t="n">
         <v>6.8</v>
       </c>
       <c r="Z5" t="n">
-        <v>1.6</v>
+        <v>-1.6</v>
       </c>
       <c r="AA5" t="n">
         <v>8.800000000000001</v>
       </c>
       <c r="AB5" t="n">
-        <v>-1.04</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="6">
@@ -7960,10 +7960,10 @@
         <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.6</v>
+        <v>0.6</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.7</v>
+        <v>0.7</v>
       </c>
       <c r="G6" t="n">
         <v>36</v>
@@ -7972,7 +7972,7 @@
         <v>229</v>
       </c>
       <c r="I6" t="n">
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="J6" t="n">
         <v>26</v>
@@ -7981,55 +7981,55 @@
         <v>114</v>
       </c>
       <c r="L6" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
         <v>14</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.3</v>
+        <v>0.3</v>
       </c>
       <c r="O6" t="n">
         <v>49.2</v>
       </c>
       <c r="P6" t="n">
-        <v>1.43</v>
+        <v>-1.43</v>
       </c>
       <c r="Q6" t="n">
         <v>0.05</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.05</v>
+        <v>0.05</v>
       </c>
       <c r="S6" t="n">
         <v>0.9419999999999999</v>
       </c>
       <c r="T6" t="n">
-        <v>0.029</v>
+        <v>-0.029</v>
       </c>
       <c r="U6" t="n">
         <v>5.8</v>
       </c>
       <c r="V6" t="n">
-        <v>-1.2</v>
+        <v>1.2</v>
       </c>
       <c r="W6" t="n">
         <v>7.4</v>
       </c>
       <c r="X6" t="n">
-        <v>0.7</v>
+        <v>-0.7</v>
       </c>
       <c r="Y6" t="n">
         <v>5.8</v>
       </c>
       <c r="Z6" t="n">
-        <v>-0.7</v>
+        <v>0.7</v>
       </c>
       <c r="AA6" t="n">
         <v>13.16</v>
       </c>
       <c r="AB6" t="n">
-        <v>-2.87</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="7">
@@ -8048,10 +8048,10 @@
         <v>2.6</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.7</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="G7" t="n">
         <v>35</v>
@@ -8060,7 +8060,7 @@
         <v>17.5</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="J7" t="n">
         <v>29.2</v>
@@ -8069,55 +8069,55 @@
         <v>170.7</v>
       </c>
       <c r="L7" t="n">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="M7" t="n">
         <v>5.2</v>
       </c>
       <c r="N7" t="n">
-        <v>-2.6</v>
+        <v>2.6</v>
       </c>
       <c r="O7" t="n">
         <v>48.56</v>
       </c>
       <c r="P7" t="n">
-        <v>3.000000000000001</v>
+        <v>-3.000000000000001</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.318</v>
+        <v>0.3179999999999999</v>
       </c>
       <c r="R7" t="n">
-        <v>0.02600000000000001</v>
+        <v>-0.026</v>
       </c>
       <c r="S7" t="n">
         <v>0.834</v>
       </c>
       <c r="T7" t="n">
-        <v>0.06599999999999999</v>
+        <v>-0.06599999999999999</v>
       </c>
       <c r="U7" t="n">
         <v>7</v>
       </c>
       <c r="V7" t="n">
-        <v>1.4</v>
+        <v>-1.4</v>
       </c>
       <c r="W7" t="n">
         <v>5.2</v>
       </c>
       <c r="X7" t="n">
-        <v>0.6</v>
+        <v>-0.6</v>
       </c>
       <c r="Y7" t="n">
         <v>7.4</v>
       </c>
       <c r="Z7" t="n">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="AA7" t="n">
         <v>11.3</v>
       </c>
       <c r="AB7" t="n">
-        <v>-0.16</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="8">
@@ -8136,10 +8136,10 @@
         <v>2.4</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.4</v>
+        <v>0.4</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="G8" t="n">
         <v>27.8</v>
@@ -8148,7 +8148,7 @@
         <v>45.2</v>
       </c>
       <c r="I8" t="n">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="J8" t="n">
         <v>28</v>
@@ -8157,55 +8157,55 @@
         <v>47</v>
       </c>
       <c r="L8" t="n">
-        <v>3.8</v>
+        <v>-3.8</v>
       </c>
       <c r="M8" t="n">
         <v>6.4</v>
       </c>
       <c r="N8" t="n">
-        <v>0.4</v>
+        <v>-0.4</v>
       </c>
       <c r="O8" t="n">
         <v>44.3</v>
       </c>
       <c r="P8" t="n">
-        <v>0.7599999999999995</v>
+        <v>-0.7599999999999995</v>
       </c>
       <c r="Q8" t="n">
         <v>0.134</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.067</v>
+        <v>0.067</v>
       </c>
       <c r="S8" t="n">
         <v>0.855</v>
       </c>
       <c r="T8" t="n">
-        <v>0.042</v>
+        <v>0.01400000000000001</v>
       </c>
       <c r="U8" t="n">
         <v>4.2</v>
       </c>
       <c r="V8" t="n">
-        <v>-2.5</v>
+        <v>2.5</v>
       </c>
       <c r="W8" t="n">
         <v>6.4</v>
       </c>
       <c r="X8" t="n">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="Y8" t="n">
         <v>4.8</v>
       </c>
       <c r="Z8" t="n">
-        <v>-0.6</v>
+        <v>0.6</v>
       </c>
       <c r="AA8" t="n">
         <v>12.7</v>
       </c>
       <c r="AB8" t="n">
-        <v>-3.24</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="9">
@@ -8224,10 +8224,10 @@
         <v>4.6</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1</v>
+        <v>-0.1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="G9" t="n">
         <v>25.8</v>
@@ -8236,7 +8236,7 @@
         <v>18.2</v>
       </c>
       <c r="I9" t="n">
-        <v>-1.7</v>
+        <v>1.7</v>
       </c>
       <c r="J9" t="n">
         <v>36</v>
@@ -8245,55 +8245,55 @@
         <v>193.5</v>
       </c>
       <c r="L9" t="n">
-        <v>3.6</v>
+        <v>-3.6</v>
       </c>
       <c r="M9" t="n">
         <v>12.4</v>
       </c>
       <c r="N9" t="n">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="O9" t="n">
         <v>47.8</v>
       </c>
       <c r="P9" t="n">
-        <v>-6.94</v>
+        <v>6.94</v>
       </c>
       <c r="Q9" t="n">
         <v>0.05</v>
       </c>
       <c r="R9" t="n">
-        <v>0.06000000000000001</v>
+        <v>-0.04666666666666668</v>
       </c>
       <c r="S9" t="n">
         <v>0.748</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.066</v>
+        <v>0.066</v>
       </c>
       <c r="U9" t="n">
         <v>3.8</v>
       </c>
       <c r="V9" t="n">
-        <v>0.3</v>
+        <v>-0.3</v>
       </c>
       <c r="W9" t="n">
         <v>14.6</v>
       </c>
       <c r="X9" t="n">
-        <v>-8.4</v>
+        <v>8.4</v>
       </c>
       <c r="Y9" t="n">
         <v>9.800000000000001</v>
       </c>
       <c r="Z9" t="n">
-        <v>-5.199999999999999</v>
+        <v>5.2</v>
       </c>
       <c r="AA9" t="n">
         <v>3.74</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.53</v>
+        <v>-0.5299999999999999</v>
       </c>
     </row>
     <row r="10">
@@ -8312,10 +8312,10 @@
         <v>4</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="G10" t="n">
         <v>32</v>
@@ -8324,7 +8324,7 @@
         <v>64</v>
       </c>
       <c r="I10" t="n">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
       <c r="J10" t="n">
         <v>27.4</v>
@@ -8333,55 +8333,55 @@
         <v>8.299999999999999</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="M10" t="n">
         <v>16.6</v>
       </c>
       <c r="N10" t="n">
-        <v>1.2</v>
+        <v>-1.2</v>
       </c>
       <c r="O10" t="n">
-        <v>51.67999999999999</v>
+        <v>51.68000000000001</v>
       </c>
       <c r="P10" t="n">
-        <v>-1.849999999999999</v>
+        <v>1.849999999999999</v>
       </c>
       <c r="Q10" t="n">
         <v>0.136</v>
       </c>
       <c r="R10" t="n">
-        <v>0.017</v>
+        <v>-0.017</v>
       </c>
       <c r="S10" t="n">
-        <v>0.8939999999999999</v>
+        <v>0.8940000000000001</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.08599999999999999</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="U10" t="n">
         <v>2.8</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.6</v>
+        <v>0.6</v>
       </c>
       <c r="W10" t="n">
         <v>6.6</v>
       </c>
       <c r="X10" t="n">
-        <v>1.4</v>
+        <v>-1.4</v>
       </c>
       <c r="Y10" t="n">
         <v>11</v>
       </c>
       <c r="Z10" t="n">
-        <v>-0.6</v>
+        <v>0.6</v>
       </c>
       <c r="AA10" t="n">
         <v>11</v>
       </c>
       <c r="AB10" t="n">
-        <v>-1.01</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="11">
@@ -8400,10 +8400,10 @@
         <v>2.4</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.5</v>
+        <v>0.4999999999999999</v>
       </c>
       <c r="G11" t="n">
         <v>32.6</v>
@@ -8412,7 +8412,7 @@
         <v>105.3</v>
       </c>
       <c r="I11" t="n">
-        <v>-2.4</v>
+        <v>2.4</v>
       </c>
       <c r="J11" t="n">
         <v>32</v>
@@ -8421,55 +8421,55 @@
         <v>50.5</v>
       </c>
       <c r="L11" t="n">
-        <v>-2.3</v>
+        <v>2.3</v>
       </c>
       <c r="M11" t="n">
         <v>26</v>
       </c>
       <c r="N11" t="n">
-        <v>-5.2</v>
+        <v>5.2</v>
       </c>
       <c r="O11" t="n">
         <v>46.6</v>
       </c>
       <c r="P11" t="n">
-        <v>-1.310000000000001</v>
+        <v>1.310000000000001</v>
       </c>
       <c r="Q11" t="n">
         <v>0.16</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.05</v>
+        <v>0.05</v>
       </c>
       <c r="S11" t="n">
         <v>0.866</v>
       </c>
       <c r="T11" t="n">
-        <v>0.067</v>
+        <v>-0.067</v>
       </c>
       <c r="U11" t="n">
         <v>14.6</v>
       </c>
       <c r="V11" t="n">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="W11" t="n">
         <v>5.4</v>
       </c>
       <c r="X11" t="n">
-        <v>-0.9</v>
+        <v>0.9</v>
       </c>
       <c r="Y11" t="n">
         <v>7</v>
       </c>
       <c r="Z11" t="n">
-        <v>-0.6</v>
+        <v>0.6</v>
       </c>
       <c r="AA11" t="n">
         <v>7.32</v>
       </c>
       <c r="AB11" t="n">
-        <v>1.42</v>
+        <v>-1.42</v>
       </c>
     </row>
     <row r="12">
@@ -8488,10 +8488,10 @@
         <v>2.8</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1</v>
+        <v>-0.1</v>
       </c>
       <c r="F12" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
         <v>37.2</v>
@@ -8500,7 +8500,7 @@
         <v>69.69999999999999</v>
       </c>
       <c r="I12" t="n">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="J12" t="n">
         <v>29.2</v>
@@ -8509,55 +8509,55 @@
         <v>33.2</v>
       </c>
       <c r="L12" t="n">
-        <v>0.4</v>
+        <v>-0.4</v>
       </c>
       <c r="M12" t="n">
         <v>14.4</v>
       </c>
       <c r="N12" t="n">
-        <v>-1.7</v>
+        <v>1.7</v>
       </c>
       <c r="O12" t="n">
         <v>50.23999999999999</v>
       </c>
       <c r="P12" t="n">
-        <v>-5.480000000000001</v>
+        <v>5.480000000000001</v>
       </c>
       <c r="Q12" t="n">
         <v>0.182</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.016</v>
+        <v>0.016</v>
       </c>
       <c r="S12" t="n">
         <v>0.766</v>
       </c>
       <c r="T12" t="n">
-        <v>0.017</v>
+        <v>-0.017</v>
       </c>
       <c r="U12" t="n">
         <v>5.4</v>
       </c>
       <c r="V12" t="n">
-        <v>1.2</v>
+        <v>-1.2</v>
       </c>
       <c r="W12" t="n">
         <v>8.4</v>
       </c>
       <c r="X12" t="n">
-        <v>0.8</v>
+        <v>-0.8</v>
       </c>
       <c r="Y12" t="n">
         <v>7.6</v>
       </c>
       <c r="Z12" t="n">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="AA12" t="n">
         <v>6.279999999999999</v>
       </c>
       <c r="AB12" t="n">
-        <v>1.39</v>
+        <v>-1.39</v>
       </c>
     </row>
     <row r="13">
@@ -8576,10 +8576,10 @@
         <v>1.6</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.6</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="G13" t="n">
         <v>25.6</v>
@@ -8588,7 +8588,7 @@
         <v>37.8</v>
       </c>
       <c r="I13" t="n">
-        <v>3.2</v>
+        <v>-3.2</v>
       </c>
       <c r="J13" t="n">
         <v>26.4</v>
@@ -8597,55 +8597,55 @@
         <v>21.3</v>
       </c>
       <c r="L13" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="M13" t="n">
         <v>14.4</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.9</v>
+        <v>0.9</v>
       </c>
       <c r="O13" t="n">
-        <v>52.62</v>
+        <v>52.61999999999999</v>
       </c>
       <c r="P13" t="n">
-        <v>3.42</v>
+        <v>-3.42</v>
       </c>
       <c r="Q13" t="n">
         <v>0.414</v>
       </c>
       <c r="R13" t="n">
-        <v>0.05400000000000001</v>
+        <v>-0.05400000000000001</v>
       </c>
       <c r="S13" t="n">
         <v>0.7875</v>
       </c>
       <c r="T13" t="n">
-        <v>0.121</v>
+        <v>-0.183</v>
       </c>
       <c r="U13" t="n">
         <v>4.2</v>
       </c>
       <c r="V13" t="n">
-        <v>0.4</v>
+        <v>-0.4</v>
       </c>
       <c r="W13" t="n">
         <v>4.6</v>
       </c>
       <c r="X13" t="n">
-        <v>-2.4</v>
+        <v>2.4</v>
       </c>
       <c r="Y13" t="n">
         <v>6</v>
       </c>
       <c r="Z13" t="n">
-        <v>-1.2</v>
+        <v>1.2</v>
       </c>
       <c r="AA13" t="n">
         <v>13.04</v>
       </c>
       <c r="AB13" t="n">
-        <v>-3.13</v>
+        <v>3.13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>